<commit_message>
added new map with door
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="4780" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="207">
   <si>
     <t>amulet</t>
   </si>
@@ -167,9 +167,6 @@
     <t>leather</t>
   </si>
   <si>
-    <t>bracers</t>
-  </si>
-  <si>
     <t>wrist</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
   </si>
   <si>
     <t>weapon</t>
-  </si>
-  <si>
-    <t>hand</t>
   </si>
   <si>
     <t>damage type, bleeding, attack speed, extra damage, socket</t>
@@ -602,15 +596,6 @@
     <t>platePants</t>
   </si>
   <si>
-    <t>leatherArmBands</t>
-  </si>
-  <si>
-    <t>mailBracers</t>
-  </si>
-  <si>
-    <t>plateBracers</t>
-  </si>
-  <si>
     <t>slippers</t>
   </si>
   <si>
@@ -687,6 +672,45 @@
   </si>
   <si>
     <t>1d3+2</t>
+  </si>
+  <si>
+    <t>gloves</t>
+  </si>
+  <si>
+    <t>laceGloves</t>
+  </si>
+  <si>
+    <t>leatherGloves</t>
+  </si>
+  <si>
+    <t>plateGloves</t>
+  </si>
+  <si>
+    <t>spriteRow</t>
+  </si>
+  <si>
+    <t>spriteCol</t>
+  </si>
+  <si>
+    <t>scarf</t>
+  </si>
+  <si>
+    <t>cloak</t>
+  </si>
+  <si>
+    <t>leatherCloak</t>
+  </si>
+  <si>
+    <t>clothCloak</t>
+  </si>
+  <si>
+    <t>mailCloak</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>mail</t>
   </si>
 </sst>
 </file>
@@ -778,8 +802,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -847,7 +877,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -877,6 +907,9 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -906,6 +939,9 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1238,7 +1274,7 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1255,40 +1291,44 @@
   <sheetData>
     <row r="1" spans="1:20" ht="16">
       <c r="A1" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -1302,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1344,13 +1384,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1386,13 +1426,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1424,16 +1464,39 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="16">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
@@ -1444,16 +1507,16 @@
     </row>
     <row r="6" spans="1:20" ht="16">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>0.1</v>
@@ -1486,16 +1549,16 @@
     </row>
     <row r="7" spans="1:20" ht="16">
       <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
         <v>0.1</v>
@@ -1510,13 +1573,13 @@
         <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1550,13 +1613,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1">
         <v>0.1</v>
@@ -1592,13 +1655,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1">
         <v>1.1000000000000001</v>
@@ -1619,7 +1682,7 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1634,13 +1697,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1">
         <v>2.1</v>
@@ -1695,13 +1758,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1719,7 +1782,7 @@
         <v>5</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>5</v>
@@ -1737,13 +1800,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1761,7 +1824,7 @@
         <v>11</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>11</v>
@@ -1779,13 +1842,13 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1803,10 +1866,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1840,10 +1903,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
@@ -1882,10 +1945,10 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
@@ -1924,10 +1987,10 @@
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
@@ -1966,10 +2029,10 @@
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>9</v>
@@ -2043,13 +2106,13 @@
     </row>
     <row r="23" spans="1:18" ht="16">
       <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -2067,13 +2130,13 @@
         <v>19</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2085,13 +2148,13 @@
     </row>
     <row r="24" spans="1:18" ht="16">
       <c r="A24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
@@ -2109,13 +2172,13 @@
         <v>18</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2127,13 +2190,13 @@
     </row>
     <row r="25" spans="1:18" ht="16">
       <c r="A25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
@@ -2154,7 +2217,7 @@
         <v>5</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>25</v>
+        <v>194</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>5</v>
@@ -2168,16 +2231,39 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" spans="1:18" ht="16">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="A26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -2187,16 +2273,39 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" ht="16">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="A27" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -2206,16 +2315,39 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" ht="16">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+      <c r="A28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F28" s="1">
+        <v>4</v>
+      </c>
+      <c r="G28" s="1">
+        <v>3</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -2226,16 +2358,16 @@
     </row>
     <row r="29" spans="1:18" ht="16">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="D29" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2253,7 +2385,7 @@
         <v>11</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>11</v>
@@ -2268,16 +2400,16 @@
     </row>
     <row r="30" spans="1:18" ht="16">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E30" s="1">
         <v>2</v>
@@ -2295,7 +2427,7 @@
         <v>24</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>24</v>
@@ -2310,16 +2442,16 @@
     </row>
     <row r="31" spans="1:18" ht="16">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E31" s="1">
         <v>3</v>
@@ -2337,7 +2469,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>5</v>
@@ -2352,16 +2484,16 @@
     </row>
     <row r="32" spans="1:18" ht="16">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -2379,7 +2511,7 @@
         <v>5</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>5</v>
@@ -2413,16 +2545,16 @@
     </row>
     <row r="34" spans="1:30" ht="16">
       <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1">
@@ -2435,7 +2567,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>13</v>
@@ -31930,342 +32062,324 @@
   <dimension ref="A1:X87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:Q1"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:19" ht="16">
+    <row r="1" spans="1:18" ht="16">
       <c r="A1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>98</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" ht="16">
+    </row>
+    <row r="2" spans="1:18" ht="16">
       <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2</v>
+      </c>
+      <c r="F2" s="4">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="M2" s="4">
+        <v>1</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="4">
+        <v>2</v>
+      </c>
+      <c r="P2" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="16">
+      <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="J3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O3" s="4">
+        <v>1</v>
+      </c>
+      <c r="P3" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="16">
+      <c r="A4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="16">
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E5" s="4">
         <v>2</v>
       </c>
-      <c r="G2" s="4">
+      <c r="F5" s="4">
         <v>3</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="N2" s="4">
-        <v>1</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="P2" s="4">
+      <c r="L5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O5" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P5" s="4">
         <v>2</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="1:18" ht="16">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" ht="16">
-      <c r="A3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="J6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="N3" s="4">
-        <v>1</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="P3" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="4">
+      <c r="L6" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="M6" s="4">
         <v>4</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" ht="16">
-      <c r="A4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="N4" s="4">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="P4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>6</v>
-      </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" ht="16">
-      <c r="A5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="N6" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O6" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P6" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="N5" s="4">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P5" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>2</v>
-      </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-    </row>
-    <row r="6" spans="1:19" ht="16">
-      <c r="A6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="F6" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="N6" s="4">
-        <v>4</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P6" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" ht="16">
+    </row>
+    <row r="7" spans="1:18" ht="16">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -32284,229 +32398,216 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" ht="16">
+    </row>
+    <row r="8" spans="1:18" ht="16">
       <c r="A8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
+      <c r="D8" s="4">
+        <v>0.1</v>
       </c>
       <c r="E8" s="4">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M8" s="4">
+        <v>1</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O8" s="4">
+        <v>1</v>
+      </c>
+      <c r="P8" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:18" ht="16">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E9" s="4">
         <v>2</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="F9" s="4">
+        <v>7</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="N8" s="4">
-        <v>1</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="P8" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>6</v>
-      </c>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-    </row>
-    <row r="9" spans="1:19" ht="16">
-      <c r="A9" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F9" s="4">
-        <v>2</v>
-      </c>
-      <c r="G9" s="4">
-        <v>7</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="I9" s="4" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>49</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="N9" s="4">
+        <v>182</v>
+      </c>
+      <c r="M9" s="4">
         <v>0</v>
       </c>
-      <c r="O9" s="4" t="s">
+      <c r="N9" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O9" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="1:18" ht="16">
+      <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="4">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="P9" s="4">
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O10" s="4">
         <v>-2</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="P10" s="4">
         <v>2</v>
       </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-    </row>
-    <row r="10" spans="1:19" ht="16">
-      <c r="A10" s="4" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" ht="16">
+      <c r="A11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="D11" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="F11" s="4">
         <v>7</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="N10" s="4">
+      <c r="I11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="M11" s="4">
         <v>0</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P10" s="4">
+      <c r="N11" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O11" s="4">
         <v>-2</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="P11" s="4">
         <v>2</v>
       </c>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
-    </row>
-    <row r="11" spans="1:19" ht="16">
-      <c r="A11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="G11" s="4">
-        <v>7</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P11" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-    </row>
-    <row r="12" spans="1:19" ht="16">
+    </row>
+    <row r="12" spans="1:18" ht="16">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -32525,337 +32626,318 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" ht="16">
+    </row>
+    <row r="13" spans="1:18" ht="16">
       <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="D13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
+        <v>5</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4">
+      <c r="K13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O13" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P13" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="16">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O14" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P14" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="16">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4">
+        <v>10</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="16">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="4">
+        <v>6</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="4" t="s">
+      <c r="H16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="N13" s="4">
+      <c r="L16" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="M16" s="4">
         <v>0</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P13" s="4">
+      <c r="N16" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O16" s="4">
         <v>-2</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="P16" s="4">
         <v>2</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" ht="16">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F14" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>3</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="N14" s="4">
-        <v>0</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P14" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q14" s="4">
-        <v>2</v>
-      </c>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" ht="16">
-      <c r="A15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="4">
-        <v>2.1</v>
-      </c>
-      <c r="F15" s="4">
-        <v>2</v>
-      </c>
-      <c r="G15" s="4">
-        <v>10</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="N15" s="4">
-        <v>0</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="P15" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>4</v>
-      </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-    </row>
-    <row r="16" spans="1:19" ht="16">
-      <c r="A16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="G16" s="4">
-        <v>6</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="N16" s="4">
-        <v>0</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="P16" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q16" s="4">
-        <v>2</v>
-      </c>
+      <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
     </row>
     <row r="17" spans="1:24" ht="16">
       <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>37</v>
+      <c r="D17" s="4">
+        <v>4.0999999999999996</v>
       </c>
       <c r="E17" s="4">
-        <v>4.0999999999999996</v>
+        <v>1.5</v>
       </c>
       <c r="F17" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="G17" s="4">
         <v>6</v>
       </c>
+      <c r="G17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="H17" s="4" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="L17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="N17" s="4">
+        <v>188</v>
+      </c>
+      <c r="M17" s="4">
         <v>0</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>183</v>
+      <c r="N17" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O17" s="4">
+        <v>-2</v>
       </c>
       <c r="P17" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q17" s="4">
         <v>2</v>
       </c>
+      <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
     </row>
     <row r="18" spans="1:24" ht="16">
       <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
+      <c r="D18" s="4">
+        <v>5.0999999999999996</v>
       </c>
       <c r="E18" s="4">
-        <v>5.0999999999999996</v>
+        <v>1.75</v>
       </c>
       <c r="F18" s="4">
-        <v>1.75</v>
-      </c>
-      <c r="G18" s="4">
         <v>4</v>
       </c>
+      <c r="G18" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="J18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K18" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="L18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="N18" s="4">
+        <v>189</v>
+      </c>
+      <c r="M18" s="4">
         <v>0</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>183</v>
+      <c r="N18" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O18" s="4">
+        <v>-2</v>
       </c>
       <c r="P18" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q18" s="4">
         <v>2</v>
       </c>
+      <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
     </row>
     <row r="19" spans="1:24" ht="16">
       <c r="A19" s="4"/>
@@ -32876,62 +32958,58 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
     </row>
     <row r="20" spans="1:24" ht="16">
       <c r="A20" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.1</v>
       </c>
       <c r="E20" s="4">
-        <v>0.1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="4">
-        <v>2</v>
+      <c r="G20" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="N20" s="4">
+        <v>178</v>
+      </c>
+      <c r="M20" s="4">
         <v>0</v>
       </c>
-      <c r="O20" s="4" t="s">
-        <v>183</v>
+      <c r="N20" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="O20" s="4">
+        <v>-2</v>
       </c>
       <c r="P20" s="4">
-        <v>-2</v>
-      </c>
-      <c r="Q20" s="4">
         <v>2</v>
       </c>
+      <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
     </row>
     <row r="21" spans="1:24" ht="16">
       <c r="A21" s="4"/>
@@ -33367,16 +33445,16 @@
   <sheetData>
     <row r="1" spans="1:21" ht="16">
       <c r="A1" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
@@ -33398,13 +33476,13 @@
     </row>
     <row r="2" spans="1:21" ht="16">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
@@ -33429,13 +33507,13 @@
     </row>
     <row r="3" spans="1:21" ht="16">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
@@ -33460,13 +33538,13 @@
     </row>
     <row r="4" spans="1:21" ht="16">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
@@ -33491,13 +33569,13 @@
     </row>
     <row r="5" spans="1:21" ht="16">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>13</v>
@@ -33522,13 +33600,13 @@
     </row>
     <row r="6" spans="1:21" ht="16">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -33553,13 +33631,13 @@
     </row>
     <row r="7" spans="1:21" ht="16">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>13</v>
@@ -33584,13 +33662,13 @@
     </row>
     <row r="8" spans="1:21" ht="16">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>13</v>
@@ -33637,16 +33715,16 @@
     </row>
     <row r="10" spans="1:21" ht="16">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -33668,16 +33746,16 @@
     </row>
     <row r="11" spans="1:21" ht="16">
       <c r="A11" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -33699,16 +33777,16 @@
     </row>
     <row r="12" spans="1:21" ht="16">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -33730,16 +33808,16 @@
     </row>
     <row r="13" spans="1:21" ht="16">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -33761,16 +33839,16 @@
     </row>
     <row r="14" spans="1:21" ht="16">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -33792,16 +33870,16 @@
     </row>
     <row r="15" spans="1:21" ht="16">
       <c r="A15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -33823,16 +33901,16 @@
     </row>
     <row r="16" spans="1:21" ht="16">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -33854,16 +33932,16 @@
     </row>
     <row r="17" spans="1:21" ht="16">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -33885,16 +33963,16 @@
     </row>
     <row r="18" spans="1:21" ht="16">
       <c r="A18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -33916,16 +33994,16 @@
     </row>
     <row r="19" spans="1:21" ht="16">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -33947,16 +34025,16 @@
     </row>
     <row r="20" spans="1:21" ht="16">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -34320,19 +34398,19 @@
   <sheetData>
     <row r="1" spans="1:20" ht="16">
       <c r="A1" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -34352,13 +34430,13 @@
     </row>
     <row r="2" spans="1:20" ht="16">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4">
         <v>4</v>
@@ -34384,13 +34462,13 @@
     </row>
     <row r="3" spans="1:20" ht="16">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -34416,13 +34494,13 @@
     </row>
     <row r="4" spans="1:20" ht="16">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
@@ -34448,13 +34526,13 @@
     </row>
     <row r="5" spans="1:20" ht="16">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -34480,13 +34558,13 @@
     </row>
     <row r="6" spans="1:20" ht="16">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -34512,13 +34590,13 @@
     </row>
     <row r="7" spans="1:20" ht="16">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -34544,13 +34622,13 @@
     </row>
     <row r="8" spans="1:20" ht="16">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -34576,13 +34654,13 @@
     </row>
     <row r="9" spans="1:20" ht="16">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -34608,13 +34686,13 @@
     </row>
     <row r="10" spans="1:20" ht="16">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
refactored level. removed game objects. created basicObjects. status has inventory. items can be picked up. no longer draw from tiled data or load directly from tiled data except walls. pretty baller yo
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
     <sheet name="weapons" sheetId="2" r:id="rId2"/>
     <sheet name="books" sheetId="4" r:id="rId3"/>
     <sheet name="misc" sheetId="3" r:id="rId4"/>
+    <sheet name="door" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="209">
   <si>
     <t>amulet</t>
   </si>
@@ -158,16 +159,7 @@
     <t>head</t>
   </si>
   <si>
-    <t>pants</t>
-  </si>
-  <si>
-    <t>leg armor</t>
-  </si>
-  <si>
     <t>leather</t>
-  </si>
-  <si>
-    <t>wrist</t>
   </si>
   <si>
     <t>strangulates, reflection, healing, life saving, unchanging, resistances, socket</t>
@@ -258,9 +250,6 @@
   </si>
   <si>
     <t>hammer</t>
-  </si>
-  <si>
-    <t>large weapon, knockback</t>
   </si>
   <si>
     <t>rock</t>
@@ -560,9 +549,6 @@
     <t>ironAmulet</t>
   </si>
   <si>
-    <t>silverAmulet</t>
-  </si>
-  <si>
     <t>shirt</t>
   </si>
   <si>
@@ -578,24 +564,6 @@
     <t>ironHelm</t>
   </si>
   <si>
-    <t>paperHat</t>
-  </si>
-  <si>
-    <t>goldCrown</t>
-  </si>
-  <si>
-    <t>satinPants</t>
-  </si>
-  <si>
-    <t>leatherChaps</t>
-  </si>
-  <si>
-    <t>mailLeggings</t>
-  </si>
-  <si>
-    <t>platePants</t>
-  </si>
-  <si>
     <t>slippers</t>
   </si>
   <si>
@@ -603,12 +571,6 @@
   </si>
   <si>
     <t>mailBoots</t>
-  </si>
-  <si>
-    <t>plateBoots</t>
-  </si>
-  <si>
-    <t>legs</t>
   </si>
   <si>
     <t>feet</t>
@@ -677,9 +639,6 @@
     <t>gloves</t>
   </si>
   <si>
-    <t>laceGloves</t>
-  </si>
-  <si>
     <t>leatherGloves</t>
   </si>
   <si>
@@ -711,6 +670,54 @@
   </si>
   <si>
     <t>mail</t>
+  </si>
+  <si>
+    <t>necklace</t>
+  </si>
+  <si>
+    <t>headband</t>
+  </si>
+  <si>
+    <t>vikingHelm</t>
+  </si>
+  <si>
+    <t>goldenGloves</t>
+  </si>
+  <si>
+    <t>powerGloves</t>
+  </si>
+  <si>
+    <t>hands</t>
+  </si>
+  <si>
+    <t>healing, resistance, attackSpeed</t>
+  </si>
+  <si>
+    <t>powerBoots</t>
+  </si>
+  <si>
+    <t>scythe</t>
+  </si>
+  <si>
+    <t>large weapon, bleeding</t>
+  </si>
+  <si>
+    <t>1d5</t>
+  </si>
+  <si>
+    <t>knockback</t>
+  </si>
+  <si>
+    <t>crossBow</t>
+  </si>
+  <si>
+    <t>attackSpeed</t>
+  </si>
+  <si>
+    <t>door</t>
+  </si>
+  <si>
+    <t>door1</t>
   </si>
 </sst>
 </file>
@@ -802,8 +809,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="65">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -877,7 +910,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="65">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -910,6 +943,19 @@
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -942,6 +988,19 @@
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1273,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1291,43 +1350,43 @@
   <sheetData>
     <row r="1" spans="1:20" ht="16">
       <c r="A1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>110</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1342,13 +1401,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -1371,8 +1430,12 @@
       <c r="K2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="L2" s="1">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1">
+        <v>16</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -1384,13 +1447,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1413,8 +1476,12 @@
       <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="L3" s="1">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <v>15</v>
+      </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -1426,13 +1493,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -1447,7 +1514,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>13</v>
@@ -1455,8 +1522,12 @@
       <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="L4" s="1">
+        <v>11</v>
+      </c>
+      <c r="M4" s="1">
+        <v>15</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1468,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -1497,8 +1568,12 @@
       <c r="K5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="L5" s="1">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1">
+        <v>8</v>
+      </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1507,16 +1582,16 @@
     </row>
     <row r="6" spans="1:20" ht="16">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1">
         <v>0.1</v>
@@ -1539,8 +1614,12 @@
       <c r="K6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="L6" s="1">
+        <v>9</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1549,16 +1628,16 @@
     </row>
     <row r="7" spans="1:20" ht="16">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1">
         <v>0.1</v>
@@ -1573,16 +1652,20 @@
         <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="L7" s="1">
+        <v>9</v>
+      </c>
+      <c r="M7" s="1">
+        <v>6</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1613,13 +1696,13 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" s="1">
         <v>0.1</v>
@@ -1642,8 +1725,12 @@
       <c r="K9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+      <c r="L9" s="1">
+        <v>10</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -1655,13 +1742,13 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" s="1">
         <v>1.1000000000000001</v>
@@ -1682,10 +1769,14 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="L10" s="1">
+        <v>10</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6</v>
+      </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1697,13 +1788,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E11" s="1">
         <v>2.1</v>
@@ -1726,8 +1817,12 @@
       <c r="K11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="L11" s="1">
+        <v>10</v>
+      </c>
+      <c r="M11" s="1">
+        <v>4</v>
+      </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1758,13 +1853,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1782,13 +1877,17 @@
         <v>5</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="L13" s="1">
+        <v>9</v>
+      </c>
+      <c r="M13" s="1">
+        <v>10</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1800,13 +1899,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1824,13 +1923,17 @@
         <v>11</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="L14" s="1">
+        <v>9</v>
+      </c>
+      <c r="M14" s="1">
+        <v>9</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1842,13 +1945,13 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1863,16 +1966,20 @@
         <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9</v>
+      </c>
+      <c r="M15" s="1">
+        <v>16</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1900,16 +2007,16 @@
     </row>
     <row r="17" spans="1:18" ht="16">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="E17" s="1">
         <v>0.1</v>
@@ -1921,19 +2028,23 @@
         <v>1</v>
       </c>
       <c r="H17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L17" s="1">
         <v>10</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="M17" s="1">
+        <v>9</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1942,40 +2053,44 @@
     </row>
     <row r="18" spans="1:18" ht="16">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="E18" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="F18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="L18" s="1">
+        <v>10</v>
+      </c>
+      <c r="M18" s="1">
+        <v>7</v>
+      </c>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1984,40 +2099,44 @@
     </row>
     <row r="19" spans="1:18" ht="16">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="E19" s="1">
         <v>2.1</v>
       </c>
       <c r="F19" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G19" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="L19" s="1">
+        <v>10</v>
+      </c>
+      <c r="M19" s="1">
+        <v>8</v>
+      </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -2026,25 +2145,25 @@
     </row>
     <row r="20" spans="1:18" ht="16">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="E20" s="1">
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G20" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>14</v>
@@ -2053,13 +2172,17 @@
         <v>5</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>23</v>
+        <v>181</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="L20" s="1">
+        <v>11</v>
+      </c>
+      <c r="M20" s="1">
+        <v>5</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -2067,18 +2190,45 @@
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" ht="16">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="A21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="1">
+        <v>10</v>
+      </c>
+      <c r="M21" s="1">
+        <v>12</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -2086,18 +2236,45 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="16">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22" s="1">
+        <v>10</v>
+      </c>
+      <c r="M22" s="1">
+        <v>15</v>
+      </c>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -2106,13 +2283,13 @@
     </row>
     <row r="23" spans="1:18" ht="16">
       <c r="A23" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>25</v>
+        <v>191</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -2121,25 +2298,29 @@
         <v>0.1</v>
       </c>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="L23" s="1">
+        <v>10</v>
+      </c>
+      <c r="M23" s="1">
+        <v>16</v>
+      </c>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2148,40 +2329,44 @@
     </row>
     <row r="24" spans="1:18" ht="16">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="E24" s="1">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="L24" s="1">
+        <v>11</v>
+      </c>
+      <c r="M24" s="1">
+        <v>6</v>
+      </c>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -2190,19 +2375,19 @@
     </row>
     <row r="25" spans="1:18" ht="16">
       <c r="A25" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>25</v>
+        <v>160</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="E25" s="1">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -2211,19 +2396,23 @@
         <v>3</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="L25" s="1">
+        <v>11</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -2232,40 +2421,44 @@
     </row>
     <row r="26" spans="1:18" ht="16">
       <c r="A26" t="s">
-        <v>201</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>202</v>
+        <v>159</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="E26" s="1">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="F26" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G26" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>201</v>
+        <v>26</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="L26" s="1">
+        <v>11</v>
+      </c>
+      <c r="M26" s="1">
+        <v>3</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -2273,41 +2466,42 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" ht="16">
-      <c r="A27" t="s">
-        <v>201</v>
-      </c>
       <c r="B27" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="E27" s="1">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="F27" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G27" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="1">
         <v>11</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="M27" s="1">
+        <v>5</v>
+      </c>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -2316,38 +2510,18 @@
     </row>
     <row r="28" spans="1:18" ht="16">
       <c r="A28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="F28" s="1">
-        <v>4</v>
-      </c>
-      <c r="G28" s="1">
-        <v>3</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -2357,41 +2531,40 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" ht="16">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>173</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
         <v>1</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="1">
         <v>11</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1">
+        <v>14</v>
+      </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
@@ -2399,39 +2572,16 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" spans="1:18" ht="16">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1">
-        <v>3</v>
-      </c>
-      <c r="G30" s="1">
-        <v>3</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -2441,39 +2591,6 @@
       <c r="R30" s="1"/>
     </row>
     <row r="31" spans="1:18" ht="16">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="1">
-        <v>3</v>
-      </c>
-      <c r="F31" s="1">
-        <v>5</v>
-      </c>
-      <c r="G31" s="1">
-        <v>5</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -2483,39 +2600,6 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18" ht="16">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="1">
-        <v>4</v>
-      </c>
-      <c r="F32" s="1">
-        <v>7</v>
-      </c>
-      <c r="G32" s="1">
-        <v>7</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -2524,17 +2608,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:30" ht="16">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+    <row r="33" spans="12:30" ht="16">
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2543,38 +2617,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:30" ht="16">
-      <c r="A34" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>13</v>
-      </c>
+    <row r="34" spans="12:30" ht="16">
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -2583,17 +2626,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:30" ht="16">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+    <row r="35" spans="12:30" ht="16">
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -2613,13 +2646,85 @@
       <c r="AB35" s="1"/>
       <c r="AC35" s="1"/>
     </row>
-    <row r="36" spans="1:30" ht="16">
+    <row r="36" spans="12:30" ht="16">
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
+    </row>
+    <row r="91" spans="2:11" ht="16">
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+    </row>
+    <row r="92" spans="2:11" ht="16">
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+    </row>
+    <row r="93" spans="2:11" ht="16">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+      <c r="J93" s="1"/>
+      <c r="K93" s="1"/>
+    </row>
+    <row r="94" spans="2:11" ht="16">
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+    </row>
+    <row r="95" spans="2:11" ht="16">
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+    </row>
+    <row r="96" spans="2:11" ht="16">
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+      <c r="J96" s="1"/>
+      <c r="K96" s="1"/>
     </row>
     <row r="97" spans="2:32" ht="16">
       <c r="B97" s="1"/>
@@ -31258,16 +31363,6 @@
       <c r="AF964" s="1"/>
     </row>
     <row r="965" spans="2:32" ht="16">
-      <c r="B965" s="1"/>
-      <c r="C965" s="1"/>
-      <c r="D965" s="1"/>
-      <c r="E965" s="1"/>
-      <c r="F965" s="1"/>
-      <c r="G965" s="1"/>
-      <c r="H965" s="1"/>
-      <c r="I965" s="1"/>
-      <c r="J965" s="1"/>
-      <c r="K965" s="1"/>
       <c r="L965" s="1"/>
       <c r="M965" s="1"/>
       <c r="N965" s="1"/>
@@ -31291,16 +31386,6 @@
       <c r="AF965" s="1"/>
     </row>
     <row r="966" spans="2:32" ht="16">
-      <c r="B966" s="1"/>
-      <c r="C966" s="1"/>
-      <c r="D966" s="1"/>
-      <c r="E966" s="1"/>
-      <c r="F966" s="1"/>
-      <c r="G966" s="1"/>
-      <c r="H966" s="1"/>
-      <c r="I966" s="1"/>
-      <c r="J966" s="1"/>
-      <c r="K966" s="1"/>
       <c r="L966" s="1"/>
       <c r="M966" s="1"/>
       <c r="N966" s="1"/>
@@ -31324,16 +31409,6 @@
       <c r="AF966" s="1"/>
     </row>
     <row r="967" spans="2:32" ht="16">
-      <c r="B967" s="1"/>
-      <c r="C967" s="1"/>
-      <c r="D967" s="1"/>
-      <c r="E967" s="1"/>
-      <c r="F967" s="1"/>
-      <c r="G967" s="1"/>
-      <c r="H967" s="1"/>
-      <c r="I967" s="1"/>
-      <c r="J967" s="1"/>
-      <c r="K967" s="1"/>
       <c r="L967" s="1"/>
       <c r="M967" s="1"/>
       <c r="N967" s="1"/>
@@ -31357,16 +31432,6 @@
       <c r="AF967" s="1"/>
     </row>
     <row r="968" spans="2:32" ht="16">
-      <c r="B968" s="1"/>
-      <c r="C968" s="1"/>
-      <c r="D968" s="1"/>
-      <c r="E968" s="1"/>
-      <c r="F968" s="1"/>
-      <c r="G968" s="1"/>
-      <c r="H968" s="1"/>
-      <c r="I968" s="1"/>
-      <c r="J968" s="1"/>
-      <c r="K968" s="1"/>
       <c r="L968" s="1"/>
       <c r="M968" s="1"/>
       <c r="N968" s="1"/>
@@ -31390,16 +31455,6 @@
       <c r="AF968" s="1"/>
     </row>
     <row r="969" spans="2:32" ht="16">
-      <c r="B969" s="1"/>
-      <c r="C969" s="1"/>
-      <c r="D969" s="1"/>
-      <c r="E969" s="1"/>
-      <c r="F969" s="1"/>
-      <c r="G969" s="1"/>
-      <c r="H969" s="1"/>
-      <c r="I969" s="1"/>
-      <c r="J969" s="1"/>
-      <c r="K969" s="1"/>
       <c r="L969" s="1"/>
       <c r="M969" s="1"/>
       <c r="N969" s="1"/>
@@ -31423,16 +31478,6 @@
       <c r="AF969" s="1"/>
     </row>
     <row r="970" spans="2:32" ht="16">
-      <c r="B970" s="1"/>
-      <c r="C970" s="1"/>
-      <c r="D970" s="1"/>
-      <c r="E970" s="1"/>
-      <c r="F970" s="1"/>
-      <c r="G970" s="1"/>
-      <c r="H970" s="1"/>
-      <c r="I970" s="1"/>
-      <c r="J970" s="1"/>
-      <c r="K970" s="1"/>
       <c r="L970" s="1"/>
       <c r="M970" s="1"/>
       <c r="N970" s="1"/>
@@ -32061,73 +32106,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:18" ht="16">
       <c r="A1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
+      <c r="Q1" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="2" spans="1:18" ht="16">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4">
         <v>0.1</v>
@@ -32145,22 +32194,22 @@
         <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="M2" s="4">
         <v>1</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="O2" s="4">
         <v>2</v>
@@ -32168,18 +32217,22 @@
       <c r="P2" s="4">
         <v>5</v>
       </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
+      <c r="Q2" s="4">
+        <v>4</v>
+      </c>
+      <c r="R2" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:18" ht="16">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4">
         <v>1.1000000000000001</v>
@@ -32197,22 +32250,22 @@
         <v>16</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="M3" s="4">
         <v>1</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="O3" s="4">
         <v>1</v>
@@ -32220,18 +32273,22 @@
       <c r="P3" s="4">
         <v>4</v>
       </c>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="Q3" s="4">
+        <v>7</v>
+      </c>
+      <c r="R3" s="4">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="16">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4" s="4">
         <v>2.1</v>
@@ -32249,22 +32306,22 @@
         <v>16</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="O4" s="4">
         <v>0</v>
@@ -32272,18 +32329,22 @@
       <c r="P4" s="4">
         <v>6</v>
       </c>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="4">
+        <v>7</v>
+      </c>
+      <c r="R4" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="16">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" s="4">
         <v>3.1</v>
@@ -32301,22 +32362,22 @@
         <v>5</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="M5" s="4">
         <v>0</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O5" s="4">
         <v>-2</v>
@@ -32324,18 +32385,22 @@
       <c r="P5" s="4">
         <v>2</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="4">
+        <v>4</v>
+      </c>
+      <c r="R5" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="16">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4">
         <v>4.0999999999999996</v>
@@ -32353,22 +32418,22 @@
         <v>5</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="M6" s="4">
         <v>4</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O6" s="4">
         <v>-2</v>
@@ -32376,8 +32441,12 @@
       <c r="P6" s="4">
         <v>2</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="Q6" s="4">
+        <v>4</v>
+      </c>
+      <c r="R6" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="16">
       <c r="A7" s="4"/>
@@ -32401,13 +32470,13 @@
     </row>
     <row r="8" spans="1:18" ht="16">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
         <v>0.1</v>
@@ -32425,22 +32494,22 @@
         <v>5</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="M8" s="4">
         <v>1</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="O8" s="4">
         <v>1</v>
@@ -32448,18 +32517,22 @@
       <c r="P8" s="4">
         <v>6</v>
       </c>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
+      <c r="Q8" s="4">
+        <v>5</v>
+      </c>
+      <c r="R8" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:18" ht="16">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="4">
         <v>1.1000000000000001</v>
@@ -32477,22 +32550,22 @@
         <v>5</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="M9" s="4">
         <v>0</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O9" s="4">
         <v>-2</v>
@@ -32500,18 +32573,22 @@
       <c r="P9" s="4">
         <v>2</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
+      <c r="Q9" s="4">
+        <v>4</v>
+      </c>
+      <c r="R9" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:18" ht="16">
       <c r="A10" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4">
         <v>2.1</v>
@@ -32529,22 +32606,22 @@
         <v>5</v>
       </c>
       <c r="I10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="K10" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O10" s="4">
         <v>-2</v>
@@ -32552,18 +32629,22 @@
       <c r="P10" s="4">
         <v>2</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
+      <c r="Q10" s="4">
+        <v>4</v>
+      </c>
+      <c r="R10" s="4">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:18" ht="16">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4">
         <v>3.1</v>
@@ -32581,22 +32662,22 @@
         <v>5</v>
       </c>
       <c r="I11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="K11" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="M11" s="4">
         <v>0</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O11" s="4">
         <v>-2</v>
@@ -32604,8 +32685,12 @@
       <c r="P11" s="4">
         <v>2</v>
       </c>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
+      <c r="Q11" s="4">
+        <v>4</v>
+      </c>
+      <c r="R11" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:18" ht="16">
       <c r="A12" s="4"/>
@@ -32629,13 +32714,13 @@
     </row>
     <row r="13" spans="1:18" ht="16">
       <c r="A13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4">
         <v>0.1</v>
@@ -32653,22 +32738,22 @@
         <v>16</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="M13" s="4">
         <v>0</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O13" s="4">
         <v>-2</v>
@@ -32676,18 +32761,22 @@
       <c r="P13" s="4">
         <v>2</v>
       </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="Q13" s="4">
+        <v>6</v>
+      </c>
+      <c r="R13" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:18" ht="16">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D14" s="4">
         <v>1.1000000000000001</v>
@@ -32699,47 +32788,51 @@
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>56</v>
+        <v>202</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="M14" s="4">
         <v>0</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="O14" s="4">
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="P14" s="4">
         <v>2</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="Q14" s="4">
+        <v>4</v>
+      </c>
+      <c r="R14" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:18" ht="16">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="4">
         <v>2.1</v>
@@ -32754,25 +32847,25 @@
         <v>10</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="M15" s="4">
         <v>0</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="O15" s="4">
         <v>0</v>
@@ -32780,18 +32873,22 @@
       <c r="P15" s="4">
         <v>4</v>
       </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="Q15" s="4">
+        <v>16</v>
+      </c>
+      <c r="R15" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:18" ht="16">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4">
         <v>3.1</v>
@@ -32809,22 +32906,22 @@
         <v>5</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="M16" s="4">
         <v>0</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O16" s="4">
         <v>-2</v>
@@ -32832,18 +32929,22 @@
       <c r="P16" s="4">
         <v>2</v>
       </c>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-    </row>
-    <row r="17" spans="1:24" ht="16">
+      <c r="Q16" s="4">
+        <v>6</v>
+      </c>
+      <c r="R16" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="16">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D17" s="4">
         <v>4.0999999999999996</v>
@@ -32861,22 +32962,22 @@
         <v>5</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="M17" s="4">
         <v>0</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O17" s="4">
         <v>-2</v>
@@ -32884,18 +32985,22 @@
       <c r="P17" s="4">
         <v>2</v>
       </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-    </row>
-    <row r="18" spans="1:24" ht="16">
+      <c r="Q17" s="4">
+        <v>6</v>
+      </c>
+      <c r="R17" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="16">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="4">
         <v>5.0999999999999996</v>
@@ -32913,22 +33018,22 @@
         <v>16</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="M18" s="4">
         <v>0</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O18" s="4">
         <v>-2</v>
@@ -32936,38 +33041,78 @@
       <c r="P18" s="4">
         <v>2</v>
       </c>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-    </row>
-    <row r="19" spans="1:24" ht="16">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-    </row>
-    <row r="20" spans="1:24" ht="16">
+      <c r="Q18" s="4">
+        <v>6</v>
+      </c>
+      <c r="R18" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="16">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2.1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="O19" s="4">
+        <v>-2</v>
+      </c>
+      <c r="P19" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>5</v>
+      </c>
+      <c r="R19" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" ht="16">
       <c r="A20" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D20" s="4">
         <v>0.1</v>
@@ -32994,13 +33139,13 @@
         <v>7</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="O20" s="4">
         <v>-2</v>
@@ -33008,36 +33153,75 @@
       <c r="P20" s="4">
         <v>2</v>
       </c>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-    </row>
-    <row r="21" spans="1:24" ht="16">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="Q20" s="4">
+        <v>7</v>
+      </c>
+      <c r="R20" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="16">
+      <c r="A21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4">
+        <v>4</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="M21" s="4">
+        <v>2</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="O21" s="4">
+        <v>0</v>
+      </c>
+      <c r="P21" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>7</v>
+      </c>
+      <c r="R21" s="4">
+        <v>11</v>
+      </c>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-    </row>
-    <row r="22" spans="1:24" ht="16">
+    </row>
+    <row r="22" spans="1:23" ht="16">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -33046,7 +33230,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:24" ht="16">
+    <row r="23" spans="1:23" ht="16">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -33055,7 +33239,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:24" ht="16">
+    <row r="24" spans="1:23" ht="16">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -33064,7 +33248,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:24" ht="16">
+    <row r="25" spans="1:23" ht="16">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -33073,7 +33257,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:24" ht="16">
+    <row r="26" spans="1:23" ht="16">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -33082,7 +33266,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:24" ht="16">
+    <row r="27" spans="1:23" ht="16">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -33091,7 +33275,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:24" ht="16">
+    <row r="28" spans="1:23" ht="16">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -33100,7 +33284,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:24" ht="16">
+    <row r="29" spans="1:23" ht="16">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -33109,7 +33293,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:24" ht="16">
+    <row r="30" spans="1:23" ht="16">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -33118,7 +33302,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:24" ht="16">
+    <row r="31" spans="1:23" ht="16">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -33127,7 +33311,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:24" ht="16">
+    <row r="32" spans="1:23" ht="16">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -33438,26 +33622,30 @@
   <dimension ref="A1:U76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:21" ht="16">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
@@ -33476,19 +33664,23 @@
     </row>
     <row r="2" spans="1:21" ht="16">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4">
+        <v>5</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -33507,19 +33699,23 @@
     </row>
     <row r="3" spans="1:21" ht="16">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4">
+        <v>5</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -33538,19 +33734,23 @@
     </row>
     <row r="4" spans="1:21" ht="16">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="E4" s="4">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <v>6</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -33569,19 +33769,23 @@
     </row>
     <row r="5" spans="1:21" ht="16">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="4">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -33600,19 +33804,23 @@
     </row>
     <row r="6" spans="1:21" ht="16">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -33631,19 +33839,23 @@
     </row>
     <row r="7" spans="1:21" ht="16">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="E7" s="4">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4">
+        <v>13</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -33662,19 +33874,23 @@
     </row>
     <row r="8" spans="1:21" ht="16">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -33715,19 +33931,23 @@
     </row>
     <row r="10" spans="1:21" ht="16">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
+        <v>80</v>
+      </c>
+      <c r="E10" s="4">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>11</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -33746,19 +33966,23 @@
     </row>
     <row r="11" spans="1:21" ht="16">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+        <v>81</v>
+      </c>
+      <c r="E11" s="4">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4">
+        <v>12</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -33777,19 +34001,23 @@
     </row>
     <row r="12" spans="1:21" ht="16">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="E12" s="4">
+        <v>16</v>
+      </c>
+      <c r="F12" s="4">
+        <v>13</v>
+      </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -33808,19 +34036,23 @@
     </row>
     <row r="13" spans="1:21" ht="16">
       <c r="A13" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="E13" s="4">
+        <v>16</v>
+      </c>
+      <c r="F13" s="4">
+        <v>11</v>
+      </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -33839,19 +34071,23 @@
     </row>
     <row r="14" spans="1:21" ht="16">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+        <v>84</v>
+      </c>
+      <c r="E14" s="4">
+        <v>16</v>
+      </c>
+      <c r="F14" s="4">
+        <v>12</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -33870,19 +34106,23 @@
     </row>
     <row r="15" spans="1:21" ht="16">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="E15" s="4">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4">
+        <v>13</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -33901,19 +34141,23 @@
     </row>
     <row r="16" spans="1:21" ht="16">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="E16" s="4">
+        <v>16</v>
+      </c>
+      <c r="F16" s="4">
+        <v>11</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -33932,19 +34176,23 @@
     </row>
     <row r="17" spans="1:21" ht="16">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="E17" s="4">
+        <v>16</v>
+      </c>
+      <c r="F17" s="4">
+        <v>12</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -33963,19 +34211,23 @@
     </row>
     <row r="18" spans="1:21" ht="16">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="E18" s="4">
+        <v>16</v>
+      </c>
+      <c r="F18" s="4">
+        <v>13</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -33994,19 +34246,23 @@
     </row>
     <row r="19" spans="1:21" ht="16">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="E19" s="4">
+        <v>16</v>
+      </c>
+      <c r="F19" s="4">
+        <v>11</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -34025,19 +34281,23 @@
     </row>
     <row r="20" spans="1:21" ht="16">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="E20" s="4">
+        <v>16</v>
+      </c>
+      <c r="F20" s="4">
+        <v>12</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -34378,6 +34638,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -34388,32 +34649,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:20" ht="16">
       <c r="A1" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -34430,13 +34695,13 @@
     </row>
     <row r="2" spans="1:20" ht="16">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4">
         <v>4</v>
@@ -34444,8 +34709,12 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -34462,13 +34731,13 @@
     </row>
     <row r="3" spans="1:20" ht="16">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D3" s="4">
         <v>0</v>
@@ -34476,8 +34745,12 @@
       <c r="E3" s="4">
         <v>2</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="F3" s="4">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4">
+        <v>8</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -34494,13 +34767,13 @@
     </row>
     <row r="4" spans="1:20" ht="16">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4">
         <v>6</v>
@@ -34508,8 +34781,12 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>12</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -34526,13 +34803,13 @@
     </row>
     <row r="5" spans="1:20" ht="16">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D5" s="4">
         <v>0</v>
@@ -34540,8 +34817,12 @@
       <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="F5" s="4">
+        <v>6</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -34558,13 +34839,13 @@
     </row>
     <row r="6" spans="1:20" ht="16">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -34572,8 +34853,12 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4">
+        <v>7</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -34590,13 +34875,13 @@
     </row>
     <row r="7" spans="1:20" ht="16">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -34604,8 +34889,12 @@
       <c r="E7" s="4">
         <v>0</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="F7" s="4">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4">
+        <v>5</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -34622,13 +34911,13 @@
     </row>
     <row r="8" spans="1:20" ht="16">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -34636,8 +34925,12 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="4">
+        <v>6</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -34654,13 +34947,13 @@
     </row>
     <row r="9" spans="1:20" ht="16">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D9" s="4">
         <v>0</v>
@@ -34668,8 +34961,12 @@
       <c r="E9" s="4">
         <v>0</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="F9" s="4">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <v>6</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -34686,19 +34983,98 @@
     </row>
     <row r="10" spans="1:20" ht="16">
       <c r="A10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="16">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>14</v>
+      </c>
+      <c r="G12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16">
+      <c r="A1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="16">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="4">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a build test for items
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="209">
   <si>
     <t>amulet</t>
   </si>
@@ -809,8 +809,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -910,7 +912,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="93">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -956,6 +958,7 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1001,6 +1004,7 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1332,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2466,6 +2470,9 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" ht="16">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>200</v>
       </c>
@@ -2509,9 +2516,6 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" spans="1:18" ht="16">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2531,6 +2535,9 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" ht="16">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
       <c r="B29" s="1" t="s">
         <v>161</v>
       </c>
@@ -34649,10 +34656,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -35002,29 +35009,6 @@
       </c>
       <c r="G10" s="4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="16">
-      <c r="A12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>14</v>
-      </c>
-      <c r="G12" s="4">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -35042,7 +35026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed door building from items
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -11,7 +11,6 @@
     <sheet name="weapons" sheetId="2" r:id="rId2"/>
     <sheet name="books" sheetId="4" r:id="rId3"/>
     <sheet name="misc" sheetId="3" r:id="rId4"/>
-    <sheet name="door" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -91,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="207">
   <si>
     <t>amulet</t>
   </si>
@@ -712,12 +711,6 @@
   </si>
   <si>
     <t>attackSpeed</t>
-  </si>
-  <si>
-    <t>door</t>
-  </si>
-  <si>
-    <t>door1</t>
   </si>
 </sst>
 </file>
@@ -35020,53 +35013,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16">
-      <c r="A1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="4"/>
-    </row>
-    <row r="2" spans="1:5" ht="16">
-      <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="4">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated items.xlsx. all items now have 'equip' property. created xml form items.xlsx
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="208">
   <si>
     <t>amulet</t>
   </si>
@@ -396,9 +396,6 @@
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>worn</t>
   </si>
   <si>
     <t>grant</t>
@@ -712,6 +709,12 @@
   <si>
     <t>attackSpeed</t>
   </si>
+  <si>
+    <t>equip</t>
+  </si>
+  <si>
+    <t>mainHand</t>
+  </si>
 </sst>
 </file>
 
@@ -802,8 +805,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -905,7 +914,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -952,6 +961,9 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -998,6 +1010,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1329,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1353,22 +1368,22 @@
         <v>100</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>106</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -1380,10 +1395,10 @@
         <v>92</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -1398,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1444,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -1490,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -1536,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -1579,10 +1594,10 @@
     </row>
     <row r="6" spans="1:20" ht="16">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -1625,10 +1640,10 @@
     </row>
     <row r="7" spans="1:20" ht="16">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1649,13 +1664,13 @@
         <v>14</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L7" s="1">
         <v>9</v>
@@ -1693,10 +1708,10 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>25</v>
@@ -1739,10 +1754,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>25</v>
@@ -1766,7 +1781,7 @@
         <v>17</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L10" s="1">
         <v>10</v>
@@ -1785,10 +1800,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
@@ -1850,13 +1865,13 @@
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1874,7 +1889,7 @@
         <v>5</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>5</v>
@@ -1896,13 +1911,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1920,7 +1935,7 @@
         <v>11</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>11</v>
@@ -1942,13 +1957,13 @@
         <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="1">
         <v>3</v>
@@ -1966,10 +1981,10 @@
         <v>5</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L15" s="1">
         <v>9</v>
@@ -2004,16 +2019,16 @@
     </row>
     <row r="17" spans="1:18" ht="16">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E17" s="1">
         <v>0.1</v>
@@ -2031,10 +2046,10 @@
         <v>2</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L17" s="1">
         <v>10</v>
@@ -2050,16 +2065,16 @@
     </row>
     <row r="18" spans="1:18" ht="16">
       <c r="A18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="C18" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E18" s="1">
         <v>1.1000000000000001</v>
@@ -2077,7 +2092,7 @@
         <v>22</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>22</v>
@@ -2096,16 +2111,16 @@
     </row>
     <row r="19" spans="1:18" ht="16">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E19" s="1">
         <v>2.1</v>
@@ -2123,7 +2138,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>5</v>
@@ -2142,16 +2157,16 @@
     </row>
     <row r="20" spans="1:18" ht="16">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -2169,7 +2184,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>5</v>
@@ -2188,13 +2203,13 @@
     </row>
     <row r="21" spans="1:18" ht="16">
       <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
@@ -2215,7 +2230,7 @@
         <v>22</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>22</v>
@@ -2234,13 +2249,13 @@
     </row>
     <row r="22" spans="1:18" ht="16">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
@@ -2261,7 +2276,7 @@
         <v>11</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>11</v>
@@ -2283,10 +2298,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
@@ -2304,10 +2319,10 @@
         <v>18</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>5</v>
@@ -2329,13 +2344,13 @@
         <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -2375,13 +2390,13 @@
         <v>26</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E25" s="1">
         <v>2</v>
@@ -2421,13 +2436,13 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -2467,13 +2482,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E27" s="1">
         <v>4</v>
@@ -2532,13 +2547,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
@@ -32106,352 +32121,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="16">
+    <row r="1" spans="1:19" ht="16">
       <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>103</v>
+      <c r="C1" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="16">
+    </row>
+    <row r="2" spans="1:19" ht="16">
       <c r="A2" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>0.1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="4">
+      <c r="M2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="N2" s="4">
         <v>1</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" s="4">
+      <c r="O2" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="4">
         <v>2</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>5</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>4</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="16">
+    <row r="3" spans="1:19" ht="16">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="M3" s="4">
+      <c r="M3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="N3" s="4">
         <v>1</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="O3" s="4">
+      <c r="O3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="P3" s="4">
         <v>1</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>4</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <v>7</v>
       </c>
-      <c r="R3" s="4">
+      <c r="S3" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="16">
+    <row r="4" spans="1:19" ht="16">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>2.1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>1.5</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M4" s="4">
+      <c r="M4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N4" s="4">
         <v>0</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="O4" s="4">
+      <c r="O4" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="P4" s="4">
         <v>0</v>
       </c>
-      <c r="P4" s="4">
+      <c r="Q4" s="4">
         <v>6</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="R4" s="4">
         <v>7</v>
       </c>
-      <c r="R4" s="4">
+      <c r="S4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="16">
+    <row r="5" spans="1:19" ht="16">
       <c r="A5" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>3.1</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="M5" s="4">
+      <c r="M5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O5" s="4">
+      <c r="O5" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P5" s="4">
         <v>-2</v>
       </c>
-      <c r="P5" s="4">
+      <c r="Q5" s="4">
         <v>2</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="R5" s="4">
         <v>4</v>
       </c>
-      <c r="R5" s="4">
+      <c r="S5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="16">
+    <row r="6" spans="1:19" ht="16">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="M6" s="4">
+      <c r="M6" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="N6" s="4">
         <v>4</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O6" s="4">
+      <c r="O6" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P6" s="4">
         <v>-2</v>
       </c>
-      <c r="P6" s="4">
+      <c r="Q6" s="4">
         <v>2</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="R6" s="4">
         <v>4</v>
       </c>
-      <c r="R6" s="4">
+      <c r="S6" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16">
+    <row r="7" spans="1:19" ht="16">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -32467,235 +32499,247 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" ht="16">
+      <c r="S7" s="4"/>
+    </row>
+    <row r="8" spans="1:19" ht="16">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>0.1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="4">
+        <v>2</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="M8" s="4">
+      <c r="M8" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N8" s="4">
         <v>1</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="O8" s="4">
+      <c r="O8" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" s="4">
         <v>1</v>
       </c>
-      <c r="P8" s="4">
+      <c r="Q8" s="4">
         <v>6</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="R8" s="4">
         <v>5</v>
       </c>
-      <c r="R8" s="4">
+      <c r="S8" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="16">
+    <row r="9" spans="1:19" ht="16">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="M9" s="4">
+      <c r="M9" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="N9" s="4">
         <v>0</v>
       </c>
-      <c r="N9" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O9" s="4">
+      <c r="O9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P9" s="4">
         <v>-2</v>
       </c>
-      <c r="P9" s="4">
+      <c r="Q9" s="4">
         <v>2</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="R9" s="4">
         <v>4</v>
       </c>
-      <c r="R9" s="4">
+      <c r="S9" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="16">
+    <row r="10" spans="1:19" ht="16">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>2.1</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>1.5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>7</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="M10" s="4">
+      <c r="M10" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="N10" s="4">
         <v>0</v>
       </c>
-      <c r="N10" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O10" s="4">
+      <c r="O10" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P10" s="4">
         <v>-2</v>
       </c>
-      <c r="P10" s="4">
+      <c r="Q10" s="4">
         <v>2</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>4</v>
       </c>
       <c r="R10" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="16">
+      <c r="S10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="16">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>3.1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>1.75</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>7</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="M11" s="4">
+      <c r="M11" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="N11" s="4">
         <v>0</v>
       </c>
-      <c r="N11" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O11" s="4">
+      <c r="O11" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P11" s="4">
         <v>-2</v>
       </c>
-      <c r="P11" s="4">
+      <c r="Q11" s="4">
         <v>2</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="R11" s="4">
         <v>4</v>
       </c>
-      <c r="R11" s="4">
+      <c r="S11" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="16">
+    <row r="12" spans="1:19" ht="16">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -32711,228 +32755,241 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" ht="16">
+      <c r="S12" s="4"/>
+    </row>
+    <row r="13" spans="1:19" ht="16">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>0.1</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>5</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="M13" s="4">
+      <c r="M13" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="N13" s="4">
         <v>0</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O13" s="4">
+      <c r="O13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P13" s="4">
         <v>-2</v>
       </c>
-      <c r="P13" s="4">
+      <c r="Q13" s="4">
         <v>2</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="R13" s="4">
         <v>6</v>
       </c>
-      <c r="R13" s="4">
+      <c r="S13" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16">
+    <row r="14" spans="1:19" ht="16">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F14" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="F14" s="4">
-        <v>3</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="L14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P14" s="4">
         <v>5</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="M14" s="4">
-        <v>0</v>
-      </c>
-      <c r="N14" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="O14" s="4">
-        <v>5</v>
-      </c>
-      <c r="P14" s="4">
+      <c r="Q14" s="4">
         <v>2</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="R14" s="4">
         <v>4</v>
       </c>
-      <c r="R14" s="4">
+      <c r="S14" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="16">
+    <row r="15" spans="1:19" ht="16">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>2.1</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>2</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>10</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="J15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M15" s="4">
+      <c r="M15" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N15" s="4">
         <v>0</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="O15" s="4">
+      <c r="O15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="P15" s="4">
         <v>0</v>
       </c>
-      <c r="P15" s="4">
+      <c r="Q15" s="4">
         <v>4</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="R15" s="4">
         <v>16</v>
       </c>
-      <c r="R15" s="4">
+      <c r="S15" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="16">
+    <row r="16" spans="1:19" ht="16">
       <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>3.1</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>1.5</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>6</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="J16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="M16" s="4">
+      <c r="M16" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="N16" s="4">
         <v>0</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O16" s="4">
+      <c r="O16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P16" s="4">
         <v>-2</v>
       </c>
-      <c r="P16" s="4">
+      <c r="Q16" s="4">
         <v>2</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="R16" s="4">
         <v>6</v>
       </c>
-      <c r="R16" s="4">
+      <c r="S16" s="4">
         <v>9</v>
       </c>
     </row>
@@ -32941,54 +32998,57 @@
         <v>31</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="4">
         <v>1.5</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>6</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="H17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="J17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L17" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="M17" s="4">
+      <c r="M17" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N17" s="4">
         <v>0</v>
       </c>
-      <c r="N17" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O17" s="4">
+      <c r="O17" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P17" s="4">
         <v>-2</v>
       </c>
-      <c r="P17" s="4">
+      <c r="Q17" s="4">
         <v>2</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="R17" s="4">
         <v>6</v>
       </c>
-      <c r="R17" s="4">
+      <c r="S17" s="4">
         <v>10</v>
       </c>
     </row>
@@ -32999,52 +33059,55 @@
       <c r="B18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>1.75</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>4</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="H18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="J18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="M18" s="4">
+      <c r="M18" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N18" s="4">
         <v>0</v>
       </c>
-      <c r="N18" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O18" s="4">
+      <c r="O18" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P18" s="4">
         <v>-2</v>
       </c>
-      <c r="P18" s="4">
+      <c r="Q18" s="4">
         <v>2</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="R18" s="4">
         <v>6</v>
       </c>
-      <c r="R18" s="4">
+      <c r="S18" s="4">
         <v>9</v>
       </c>
     </row>
@@ -33055,167 +33118,175 @@
       <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>2.1</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>2</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>5</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="H19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="K19" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="L19" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="M19" s="4">
+      <c r="M19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N19" s="4">
         <v>0</v>
       </c>
-      <c r="N19" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O19" s="4">
+      <c r="O19" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P19" s="4">
         <v>-2</v>
       </c>
-      <c r="P19" s="4">
+      <c r="Q19" s="4">
         <v>2</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R19" s="4">
         <v>5</v>
       </c>
-      <c r="R19" s="4">
+      <c r="S19" s="4">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="16">
       <c r="A20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>0.1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>2</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="4">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="I20" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="K20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M20" s="4">
+      <c r="M20" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N20" s="4">
         <v>0</v>
       </c>
-      <c r="N20" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O20" s="4">
+      <c r="O20" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P20" s="4">
         <v>-2</v>
       </c>
-      <c r="P20" s="4">
+      <c r="Q20" s="4">
         <v>2</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="R20" s="4">
         <v>7</v>
       </c>
-      <c r="R20" s="4">
+      <c r="S20" s="4">
         <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="16">
       <c r="A21" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C21" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="4">
+      <c r="E21" s="4">
         <v>0.1</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>2</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="K21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L21" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="M21" s="4">
+      <c r="M21" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N21" s="4">
         <v>2</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="O21" s="4">
+      <c r="O21" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P21" s="4">
         <v>0</v>
       </c>
-      <c r="P21" s="4">
+      <c r="Q21" s="4">
         <v>2</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="R21" s="4">
         <v>7</v>
       </c>
-      <c r="R21" s="4">
+      <c r="S21" s="4">
         <v>11</v>
       </c>
-      <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
@@ -33622,7 +33693,7 @@
   <dimension ref="A1:U76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33634,19 +33705,21 @@
       <c r="B1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -33664,24 +33737,26 @@
     </row>
     <row r="2" spans="1:21" ht="16">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>14</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>5</v>
       </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -33699,24 +33774,26 @@
     </row>
     <row r="3" spans="1:21" ht="16">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>5</v>
       </c>
-      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -33734,24 +33811,26 @@
     </row>
     <row r="4" spans="1:21" ht="16">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>14</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>6</v>
       </c>
-      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -33769,24 +33848,26 @@
     </row>
     <row r="5" spans="1:21" ht="16">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="4">
         <v>14</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>9</v>
       </c>
-      <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -33804,24 +33885,26 @@
     </row>
     <row r="6" spans="1:21" ht="16">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="4">
         <v>14</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>10</v>
       </c>
-      <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -33839,24 +33922,26 @@
     </row>
     <row r="7" spans="1:21" ht="16">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="4">
         <v>14</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>13</v>
       </c>
-      <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -33874,24 +33959,26 @@
     </row>
     <row r="8" spans="1:21" ht="16">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="4">
         <v>14</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -33909,7 +33996,6 @@
     </row>
     <row r="9" spans="1:21" ht="16">
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -33931,24 +34017,26 @@
     </row>
     <row r="10" spans="1:21" ht="16">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="4">
         <v>16</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>11</v>
       </c>
-      <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -33966,24 +34054,26 @@
     </row>
     <row r="11" spans="1:21" ht="16">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>16</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>12</v>
       </c>
-      <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
@@ -34001,24 +34091,26 @@
     </row>
     <row r="12" spans="1:21" ht="16">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>16</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>13</v>
       </c>
-      <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -34036,24 +34128,26 @@
     </row>
     <row r="13" spans="1:21" ht="16">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>16</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>11</v>
       </c>
-      <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -34071,24 +34165,26 @@
     </row>
     <row r="14" spans="1:21" ht="16">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C14" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>16</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>12</v>
       </c>
-      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -34106,24 +34202,26 @@
     </row>
     <row r="15" spans="1:21" ht="16">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>16</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="4">
         <v>13</v>
       </c>
-      <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
@@ -34141,24 +34239,26 @@
     </row>
     <row r="16" spans="1:21" ht="16">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>16</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>11</v>
       </c>
-      <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -34176,24 +34276,26 @@
     </row>
     <row r="17" spans="1:21" ht="16">
       <c r="A17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" t="s">
+        <v>207</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="4">
         <v>16</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>12</v>
       </c>
-      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -34211,24 +34313,26 @@
     </row>
     <row r="18" spans="1:21" ht="16">
       <c r="A18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" t="s">
+        <v>207</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>16</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>13</v>
       </c>
-      <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
@@ -34246,24 +34350,26 @@
     </row>
     <row r="19" spans="1:21" ht="16">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>16</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>11</v>
       </c>
-      <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
@@ -34281,24 +34387,26 @@
     </row>
     <row r="20" spans="1:21" ht="16">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>16</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>12</v>
       </c>
-      <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -34651,8 +34759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34664,22 +34772,24 @@
       <c r="B1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
@@ -34700,22 +34810,24 @@
       <c r="B2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
         <v>12</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="4">
         <v>2</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -34736,22 +34848,24 @@
       <c r="B3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="4">
         <v>14</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>8</v>
       </c>
-      <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -34772,22 +34886,24 @@
       <c r="B4" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="4">
         <v>12</v>
       </c>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -34806,24 +34922,26 @@
         <v>48</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
       </c>
       <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
         <v>6</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>3</v>
       </c>
-      <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -34842,24 +34960,26 @@
         <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
       </c>
       <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4">
         <v>7</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="4">
         <v>3</v>
       </c>
-      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -34878,24 +34998,26 @@
         <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
       </c>
       <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
         <v>6</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>5</v>
       </c>
-      <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -34914,24 +35036,26 @@
         <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
       </c>
       <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
         <v>6</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="4">
         <v>4</v>
       </c>
-      <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -34950,24 +35074,26 @@
         <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
       </c>
       <c r="E9" s="4">
         <v>0</v>
       </c>
       <c r="F9" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G9" s="4">
         <v>6</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4">
+        <v>6</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -34983,24 +35109,27 @@
     </row>
     <row r="10" spans="1:20" ht="16">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
       </c>
       <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
         <v>12</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="4">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed error in excel2xml.py. previously the 'type' column was called id' now it is correctly 'type'
</commit_message>
<xml_diff>
--- a/items/items.xlsx
+++ b/items/items.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
@@ -1344,7 +1344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -32121,7 +32121,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>